<commit_message>
PID Total 20 Half 30 100 Hz
</commit_message>
<xml_diff>
--- a/control_test/realTunning/D40.xlsx
+++ b/control_test/realTunning/D40.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="20 20 40" sheetId="1" r:id="rId1"/>
@@ -81,6 +81,1684 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'30 40 40'!$A$1:$A$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>12.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'30 40 40'!$C$1:$C$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-4.3633230960000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2.1816615480000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-2.1816615480000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-2.1816615480000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.4541537540000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.8174773160000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.617993951E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.945243195E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.272492439E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.8361599889999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-3.1634092330000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-9.8174773160000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-3.2724924390000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-1.418079995E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-1.7453292379999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-1.7453292379999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-1.636246219E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-1.636246219E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-1.527163107E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BC30-4740-86D1-10EBAA6DFB0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'30 40 40'!$A$1:$A$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>12.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'30 40 40'!$F$1:$F$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.0725784819999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.963495463E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.963495463E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.963495463E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.963495463E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.7453292379999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.527163107E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.527163107E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.308996975E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.090830751E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.199913863E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.199913863E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.090830774E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.090830774E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.527163107E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.3268184660000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.3268184660000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-0.1014472619</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-0.3196134269</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-0.29997846480000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.4724062090000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.617993951E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.617993951E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.617993951E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.617993951E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.617993951E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BC30-4740-86D1-10EBAA6DFB0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="365552512"/>
+        <c:axId val="365551528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="365552512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="365551528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="365551528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="365552512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2335,8 +4013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" activeCellId="2" sqref="A1:A1048576 C1:C1048576 F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4141,6 +5819,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9820,7 +11499,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I67"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13909,7 +15588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>

</xml_diff>